<commit_message>
Reflect swap of timestamp/timestamp_data_host in sheet
</commit_message>
<xml_diff>
--- a/datastatic/datasets/online/SDG9_Investment_in_R_and_D_as_%_of_GDP_OECD_2014.xlsx
+++ b/datastatic/datasets/online/SDG9_Investment_in_R_and_D_as_%_of_GDP_OECD_2014.xlsx
@@ -781,8 +781,8 @@
       <c r="A25" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="9">
-        <v>2014.0</v>
+      <c r="B25" s="14">
+        <v>42664.0</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -805,10 +805,9 @@
       <c r="A27" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="14">
-        <v>42664.0</v>
-      </c>
-      <c r="C27" s="3"/>
+      <c r="B27" s="2">
+        <v>2014.0</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>

</xml_diff>